<commit_message>
update .gitignore + xlsx file
</commit_message>
<xml_diff>
--- a/participante.xlsx
+++ b/participante.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\osrepo\Code's\Pythons-Scripts\CSV QR Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\osrepo\Programming Project\QR-code-Generator-and-checker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754911FD-3A18-4945-808C-B1C38C47A1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8808DD80-8CC8-451A-8195-59300B158B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>miranamiren@gmail.com</t>
+  </si>
+  <si>
+    <t>gmysto6@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,6 +533,9 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E4" t="s">
         <v>18</v>
       </c>
@@ -584,7 +590,9 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{025F4FDA-2AE5-4F01-9F04-8112FD9925A2}"/>
     <hyperlink ref="D5" r:id="rId3" xr:uid="{3768DAE0-D8B1-4F58-9870-B95130658EE2}"/>
     <hyperlink ref="D6" r:id="rId4" xr:uid="{5395A022-2192-4899-AF2A-3E67A832C2F6}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{F4828E02-27E8-4894-B496-BFA401400E00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>